<commit_message>
All sources working except for C&L
</commit_message>
<xml_diff>
--- a/TestCAS.xlsx
+++ b/TestCAS.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arche/Documents/Python/ARCHEscreeningTool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32D142E-1D24-F54B-A110-E4890C9B25CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1334209-E710-4242-A626-05B9143B807C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28580" yWindow="1060" windowWidth="27720" windowHeight="17440" xr2:uid="{AC7C4B23-1DA4-2B48-871A-9902A8034EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,65 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>101-84-8</t>
-  </si>
-  <si>
-    <t>202-981-2</t>
-  </si>
-  <si>
-    <t>105-21-5</t>
-  </si>
-  <si>
-    <t>203-279-9</t>
-  </si>
-  <si>
-    <t>106-22-9</t>
-  </si>
-  <si>
-    <t>203-375-0</t>
-  </si>
-  <si>
-    <t>106-68-3</t>
-  </si>
-  <si>
-    <t>203-423-0</t>
-  </si>
-  <si>
-    <t>110-43-0</t>
-  </si>
-  <si>
-    <t>203-767-1</t>
-  </si>
-  <si>
-    <t>111-13-7</t>
-  </si>
-  <si>
-    <t>203-837-1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>difenil éter</t>
-  </si>
-  <si>
-    <t>Heptan-4-olide</t>
-  </si>
-  <si>
-    <t>Citronellol</t>
-  </si>
-  <si>
-    <t>Octan-3-one</t>
-  </si>
-  <si>
-    <t>Heptan-2-one</t>
-  </si>
-  <si>
-    <t>octan-2-ona</t>
-  </si>
-  <si>
     <t>CAS</t>
   </si>
   <si>
@@ -102,13 +48,40 @@
   </si>
   <si>
     <t xml:space="preserve">413615-35-7	</t>
+  </si>
+  <si>
+    <t>1166-46-7</t>
+  </si>
+  <si>
+    <t>141-62-8</t>
+  </si>
+  <si>
+    <t>141-63-9</t>
+  </si>
+  <si>
+    <t>85877-79-8</t>
+  </si>
+  <si>
+    <t>75-09-2</t>
+  </si>
+  <si>
+    <t>597-82-0</t>
+  </si>
+  <si>
+    <t>72963-72-5</t>
+  </si>
+  <si>
+    <t>1195-32-0</t>
+  </si>
+  <si>
+    <t>215-724-4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,17 +96,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -158,7 +120,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -173,52 +135,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -245,39 +162,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -614,97 +513,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219314F5-F3E4-514C-9E76-324895DDE06E}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>14</v>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="11"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>